<commit_message>
run testcase and update
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/ProductCollection.xlsx
+++ b/src/main/resources/excels/ProductCollection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="175">
   <si>
     <t>Title</t>
   </si>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="E37" s="4"/>
       <c r="F37" t="s" s="0">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="40.200000000000003" thickBot="1">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="E52" s="4"/>
       <c r="F52" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="53.4" thickBot="1">

</xml_diff>